<commit_message>
Fix problem of hard-coded shoe size name columns.
</commit_message>
<xml_diff>
--- a/backend-python/general_document/装箱配码.xlsx
+++ b/backend-python/general_document/装箱配码.xlsx
@@ -908,7 +908,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1028,6 +1028,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1421,15 +1437,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col width="16" customWidth="1" style="37" min="21" max="21"/>
+    <col width="19" customWidth="1" style="37" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="37">
@@ -1504,7 +1520,7 @@
       <c r="T4" s="40" t="n"/>
       <c r="U4" s="33" t="inlineStr">
         <is>
-          <t>商标：XTI</t>
+          <t>商标：CLOWSE</t>
         </is>
       </c>
     </row>
@@ -1518,121 +1534,93 @@
       <c r="G5" s="41" t="n"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I5" s="12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J5" s="12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="K5" s="12" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="I5" s="12" t="inlineStr">
-        <is>
-          <t>7.5</t>
-        </is>
-      </c>
-      <c r="J5" s="12" t="inlineStr">
+      <c r="L5" s="12" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="K5" s="12" t="inlineStr">
-        <is>
-          <t>8.5</t>
-        </is>
-      </c>
-      <c r="L5" s="12" t="inlineStr">
+      <c r="M5" s="12" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="M5" s="12" t="inlineStr">
-        <is>
-          <t>9.5</t>
-        </is>
-      </c>
-      <c r="N5" s="12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="O5" s="12" t="inlineStr">
-        <is>
-          <t>10.5</t>
-        </is>
-      </c>
-      <c r="P5" s="12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="Q5" s="12" t="inlineStr">
-        <is>
-          <t>11.5</t>
-        </is>
-      </c>
-      <c r="R5" s="12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="S5" s="12" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="T5" s="12" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
+      <c r="N5" s="12" t="n"/>
+      <c r="O5" s="12" t="n"/>
+      <c r="P5" s="12" t="n"/>
+      <c r="Q5" s="12" t="n"/>
+      <c r="R5" s="12" t="n"/>
+      <c r="S5" s="12" t="n"/>
+      <c r="T5" s="12" t="n"/>
       <c r="U5" s="34" t="inlineStr">
         <is>
-          <t>备注</t>
+          <t>配码名称</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>K22-1113</t>
+          <t>K24-003</t>
         </is>
       </c>
       <c r="B6" s="15" t="n"/>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>D0229M1</t>
+          <t>2E18611</t>
         </is>
       </c>
       <c r="D6" s="17" t="n"/>
       <c r="E6" s="16" t="inlineStr">
         <is>
-          <t>test-98</t>
+          <t>173030</t>
         </is>
       </c>
       <c r="F6" s="18" t="inlineStr">
         <is>
-          <t>灰色</t>
+          <t>蓝色</t>
         </is>
       </c>
       <c r="G6" s="19" t="n">
-        <v>16000</v>
+        <v>120</v>
       </c>
       <c r="H6" s="42" t="n">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="I6" s="31" t="n">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="J6" s="31" t="n">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="K6" s="31" t="n">
-        <v>2000</v>
+        <v>30</v>
       </c>
       <c r="L6" s="31" t="n">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="M6" s="31" t="n">
-        <v>5000</v>
+        <v>10</v>
       </c>
       <c r="N6" s="31" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="31" t="n">
         <v>0</v>
@@ -1654,136 +1642,232 @@
       </c>
       <c r="U6" s="35" t="inlineStr">
         <is>
-          <t>TEMP1</t>
+          <t>S12B</t>
         </is>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="37">
-      <c r="A7" s="21" t="n"/>
-      <c r="B7" s="22" t="n"/>
-      <c r="C7" s="23" t="n"/>
-      <c r="D7" s="24" t="n"/>
-      <c r="E7" s="23" t="n"/>
-      <c r="F7" s="25" t="inlineStr">
-        <is>
-          <t>合计：</t>
-        </is>
-      </c>
-      <c r="G7" s="26">
-        <f>SUM(G6:G6)</f>
-        <v/>
-      </c>
-      <c r="H7" s="27">
-        <f>SUM(H6:H6)</f>
-        <v/>
-      </c>
-      <c r="I7" s="32">
-        <f>SUM(I6:I6)</f>
-        <v/>
-      </c>
-      <c r="J7" s="32">
-        <f>SUM(J6:J6)</f>
-        <v/>
-      </c>
-      <c r="K7" s="32">
-        <f>SUM(K6:K6)</f>
-        <v/>
-      </c>
-      <c r="L7" s="32">
-        <f>SUM(L6:L6)</f>
-        <v/>
-      </c>
-      <c r="M7" s="32">
-        <f>SUM(M6:M6)</f>
-        <v/>
-      </c>
-      <c r="N7" s="32">
-        <f>SUM(N6:N6)</f>
-        <v/>
-      </c>
-      <c r="O7" s="32">
-        <f>SUM(O6:O6)</f>
-        <v/>
-      </c>
-      <c r="P7" s="32">
-        <f>SUM(P6:P6)</f>
-        <v/>
-      </c>
-      <c r="Q7" s="32">
-        <f>SUM(Q6:Q6)</f>
-        <v/>
-      </c>
-      <c r="R7" s="32">
-        <f>SUM(R6:R6)</f>
-        <v/>
-      </c>
-      <c r="S7" s="32">
-        <f>SUM(S6:S6)</f>
-        <v/>
-      </c>
-      <c r="T7" s="32">
-        <f>SUM(T6:T6)</f>
-        <v/>
-      </c>
-      <c r="U7" s="36" t="n"/>
+      <c r="A7" s="43" t="n"/>
+      <c r="B7" s="44" t="n"/>
+      <c r="C7" s="43" t="n"/>
+      <c r="D7" s="45" t="n"/>
+      <c r="E7" s="43" t="n"/>
+      <c r="F7" s="46" t="inlineStr">
+        <is>
+          <t>白色</t>
+        </is>
+      </c>
+      <c r="G7" s="47" t="n">
+        <v>60</v>
+      </c>
+      <c r="H7" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="J7" s="46" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" s="46" t="n">
+        <v>15</v>
+      </c>
+      <c r="L7" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="M7" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="48" t="inlineStr">
+        <is>
+          <t>S12B</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="28" t="inlineStr">
-        <is>
-          <t>后处理：</t>
-        </is>
-      </c>
-      <c r="B8" s="43" t="n"/>
-      <c r="C8" s="43" t="n"/>
-      <c r="D8" s="43" t="n"/>
-      <c r="E8" s="43" t="n"/>
-      <c r="F8" s="43" t="n"/>
-      <c r="G8" s="43" t="n"/>
-      <c r="H8" s="43" t="n"/>
-      <c r="I8" s="43" t="n"/>
-      <c r="J8" s="43" t="n"/>
-      <c r="K8" s="43" t="n"/>
-      <c r="L8" s="43" t="n"/>
-      <c r="M8" s="43" t="n"/>
-      <c r="N8" s="43" t="n"/>
-      <c r="O8" s="43" t="n"/>
-      <c r="P8" s="43" t="n"/>
-      <c r="Q8" s="43" t="n"/>
-      <c r="R8" s="43" t="n"/>
-      <c r="S8" s="43" t="n"/>
-      <c r="T8" s="43" t="n"/>
-      <c r="U8" s="44" t="n"/>
+      <c r="A8" s="41" t="n"/>
+      <c r="B8" s="44" t="n"/>
+      <c r="C8" s="41" t="n"/>
+      <c r="D8" s="45" t="n"/>
+      <c r="E8" s="41" t="n"/>
+      <c r="F8" s="46" t="inlineStr">
+        <is>
+          <t>白色</t>
+        </is>
+      </c>
+      <c r="G8" s="47" t="n">
+        <v>50</v>
+      </c>
+      <c r="H8" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="J8" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="K8" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="L8" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="M8" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="N8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="48" t="inlineStr">
+        <is>
+          <t>S12C</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="37">
-      <c r="A9" s="45" t="inlineStr">
+      <c r="A9" s="21" t="n"/>
+      <c r="B9" s="22" t="n"/>
+      <c r="C9" s="23" t="n"/>
+      <c r="D9" s="24" t="n"/>
+      <c r="E9" s="23" t="n"/>
+      <c r="F9" s="25" t="inlineStr">
+        <is>
+          <t>合计：</t>
+        </is>
+      </c>
+      <c r="G9" s="26">
+        <f>SUM(G6:G8)</f>
+        <v/>
+      </c>
+      <c r="H9" s="27">
+        <f>SUM(H6:H8)</f>
+        <v/>
+      </c>
+      <c r="I9" s="32">
+        <f>SUM(I6:I8)</f>
+        <v/>
+      </c>
+      <c r="J9" s="32">
+        <f>SUM(J6:J8)</f>
+        <v/>
+      </c>
+      <c r="K9" s="32">
+        <f>SUM(K6:K8)</f>
+        <v/>
+      </c>
+      <c r="L9" s="32">
+        <f>SUM(L6:L8)</f>
+        <v/>
+      </c>
+      <c r="M9" s="32">
+        <f>SUM(M6:M8)</f>
+        <v/>
+      </c>
+      <c r="N9" s="32" t="n"/>
+      <c r="O9" s="32" t="n"/>
+      <c r="P9" s="32" t="n"/>
+      <c r="Q9" s="32" t="n"/>
+      <c r="R9" s="32" t="n"/>
+      <c r="S9" s="32" t="n"/>
+      <c r="T9" s="32" t="n"/>
+      <c r="U9" s="36" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="28" t="inlineStr">
+        <is>
+          <t>后处理：</t>
+        </is>
+      </c>
+      <c r="B10" s="49" t="n"/>
+      <c r="C10" s="49" t="n"/>
+      <c r="D10" s="49" t="n"/>
+      <c r="E10" s="49" t="n"/>
+      <c r="F10" s="49" t="n"/>
+      <c r="G10" s="49" t="n"/>
+      <c r="H10" s="49" t="n"/>
+      <c r="I10" s="49" t="n"/>
+      <c r="J10" s="49" t="n"/>
+      <c r="K10" s="49" t="n"/>
+      <c r="L10" s="49" t="n"/>
+      <c r="M10" s="49" t="n"/>
+      <c r="N10" s="49" t="n"/>
+      <c r="O10" s="49" t="n"/>
+      <c r="P10" s="49" t="n"/>
+      <c r="Q10" s="49" t="n"/>
+      <c r="R10" s="49" t="n"/>
+      <c r="S10" s="49" t="n"/>
+      <c r="T10" s="49" t="n"/>
+      <c r="U10" s="50" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="51" t="inlineStr">
         <is>
           <t>特别注意：</t>
         </is>
       </c>
-      <c r="B9" s="43" t="n"/>
-      <c r="C9" s="43" t="n"/>
-      <c r="D9" s="43" t="n"/>
-      <c r="E9" s="43" t="n"/>
-      <c r="F9" s="43" t="n"/>
-      <c r="G9" s="43" t="n"/>
-      <c r="H9" s="43" t="n"/>
-      <c r="I9" s="43" t="n"/>
-      <c r="J9" s="43" t="n"/>
-      <c r="K9" s="43" t="n"/>
-      <c r="L9" s="43" t="n"/>
-      <c r="M9" s="43" t="n"/>
-      <c r="N9" s="43" t="n"/>
-      <c r="O9" s="43" t="n"/>
-      <c r="P9" s="43" t="n"/>
-      <c r="Q9" s="43" t="n"/>
-      <c r="R9" s="43" t="n"/>
-      <c r="S9" s="43" t="n"/>
-      <c r="T9" s="43" t="n"/>
-      <c r="U9" s="44" t="n"/>
+      <c r="B11" s="49" t="n"/>
+      <c r="C11" s="49" t="n"/>
+      <c r="D11" s="49" t="n"/>
+      <c r="E11" s="49" t="n"/>
+      <c r="F11" s="49" t="n"/>
+      <c r="G11" s="49" t="n"/>
+      <c r="H11" s="49" t="n"/>
+      <c r="I11" s="49" t="n"/>
+      <c r="J11" s="49" t="n"/>
+      <c r="K11" s="49" t="n"/>
+      <c r="L11" s="49" t="n"/>
+      <c r="M11" s="49" t="n"/>
+      <c r="N11" s="49" t="n"/>
+      <c r="O11" s="49" t="n"/>
+      <c r="P11" s="49" t="n"/>
+      <c r="Q11" s="49" t="n"/>
+      <c r="R11" s="49" t="n"/>
+      <c r="S11" s="49" t="n"/>
+      <c r="T11" s="49" t="n"/>
+      <c r="U11" s="50" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="H4:T4"/>
     <mergeCell ref="A2:U2"/>
@@ -1793,12 +1877,13 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="E6"/>
-    <mergeCell ref="C6"/>
+    <mergeCell ref="A11:U11"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="A10:U10"/>
     <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A9:U9"/>
-    <mergeCell ref="A8:U8"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A3:U3"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="C6">
     <cfRule type="duplicateValues" priority="1" dxfId="0"/>

</xml_diff>